<commit_message>
refactor FURPS table in exc 2 refactor adr in exc 4
</commit_message>
<xml_diff>
--- a/Exc2/FURPS_table.xlsx
+++ b/Exc2/FURPS_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\study\archdev\ya\architecture-sprint-9\Exc2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{989D3D60-077E-47ED-A127-4E95EFBC2469}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81A83712-4BFA-44F8-B251-5FBB17843CE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
   <si>
     <t>Код</t>
   </si>
@@ -245,6 +245,42 @@
   </si>
   <si>
     <t>R+3</t>
+  </si>
+  <si>
+    <t>Использование платформ Java, .NET, PHP</t>
+  </si>
+  <si>
+    <t>Разработка должна вестись на платформах, с которыми уже есть экспертиза у сотрудников банка.</t>
+  </si>
+  <si>
+    <t>Использование существующих баз данных</t>
+  </si>
+  <si>
+    <t>Использование Oracle и MS SQL помогает снизить затраты на внедрение новых технологий.</t>
+  </si>
+  <si>
+    <t>Ограничения на масштабирование АБС</t>
+  </si>
+  <si>
+    <t>АБС может масштабироваться только вертикально, что ограничивает возможность работы с большими объёмами данных.</t>
+  </si>
+  <si>
+    <t>Ограничения безопасности</t>
+  </si>
+  <si>
+    <t>Все данные должны быть переданы по защищённым каналам, соответствующим требованиям регуляторов.</t>
+  </si>
+  <si>
+    <t>R+4</t>
+  </si>
+  <si>
+    <t>R+5</t>
+  </si>
+  <si>
+    <t>R+6</t>
+  </si>
+  <si>
+    <t>R+7</t>
   </si>
 </sst>
 </file>
@@ -299,7 +335,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -322,11 +358,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -337,15 +393,21 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -573,10 +635,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:I29"/>
+  <dimension ref="B1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29:D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.42578125" defaultRowHeight="12.75"/>
@@ -603,10 +665,10 @@
       <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="4"/>
+      <c r="D4" s="6"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -615,10 +677,10 @@
       <c r="B5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>17</v>
       </c>
       <c r="I5" s="1"/>
@@ -627,10 +689,10 @@
       <c r="B6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4" t="s">
         <v>20</v>
       </c>
       <c r="I6" s="1"/>
@@ -639,10 +701,10 @@
       <c r="B7" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="4" t="s">
         <v>23</v>
       </c>
       <c r="I7" s="1"/>
@@ -651,10 +713,10 @@
       <c r="B8" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="4" t="s">
         <v>26</v>
       </c>
     </row>
@@ -662,10 +724,10 @@
       <c r="B9" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="4" t="s">
         <v>29</v>
       </c>
     </row>
@@ -673,19 +735,19 @@
       <c r="B10" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="4"/>
+      <c r="D10" s="6"/>
     </row>
     <row r="11" spans="2:9" ht="47.25">
       <c r="B11" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="4" t="s">
         <v>32</v>
       </c>
       <c r="G11" s="1"/>
@@ -696,10 +758,10 @@
       <c r="B12" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="4" t="s">
         <v>35</v>
       </c>
       <c r="G12" s="1"/>
@@ -710,10 +772,10 @@
       <c r="B13" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="4" t="s">
         <v>38</v>
       </c>
     </row>
@@ -721,169 +783,230 @@
       <c r="B14" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="4"/>
+      <c r="D14" s="6"/>
     </row>
     <row r="15" spans="2:9" ht="31.5">
       <c r="B15" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="4" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="16" spans="2:9" ht="47.25">
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="2:4" ht="31.5">
+    <row r="17" spans="2:6" ht="31.5">
       <c r="B17" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="2:4" ht="15.75">
+    <row r="18" spans="2:6" ht="15.75">
       <c r="B18" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D18" s="4"/>
-    </row>
-    <row r="19" spans="2:4" ht="63">
+      <c r="D18" s="6"/>
+    </row>
+    <row r="19" spans="2:6" ht="63">
       <c r="B19" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="2:4" ht="63">
-      <c r="B20" s="6" t="s">
+    <row r="20" spans="2:6" ht="63">
+      <c r="B20" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="2:4" ht="31.5">
+    <row r="21" spans="2:6" ht="31.5">
       <c r="B21" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D21" s="4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="2:4" ht="15.75">
+    <row r="22" spans="2:6" ht="15.75">
       <c r="B22" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D22" s="4"/>
-    </row>
-    <row r="23" spans="2:4" ht="63">
+      <c r="D22" s="6"/>
+    </row>
+    <row r="23" spans="2:6" ht="63">
       <c r="B23" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="4" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="24" spans="2:4" ht="47.25">
-      <c r="B24" s="6" t="s">
+    <row r="24" spans="2:6" ht="47.25">
+      <c r="B24" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C24" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D24" s="4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="2:4" ht="47.25">
+    <row r="25" spans="2:6" ht="47.25">
       <c r="B25" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D25" s="4" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="26" spans="2:4" ht="15.75">
+    <row r="26" spans="2:6" ht="15.75">
       <c r="B26" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C26" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D26" s="4"/>
-    </row>
-    <row r="27" spans="2:4" ht="47.25">
+      <c r="D26" s="6"/>
+    </row>
+    <row r="27" spans="2:6" ht="47.25">
       <c r="B27" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="C27" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D27" s="4" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="28" spans="2:4" ht="47.25">
-      <c r="B28" s="6" t="s">
+    <row r="28" spans="2:6" ht="47.25">
+      <c r="B28" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C28" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D28" s="4" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="29" spans="2:4" ht="63">
+    <row r="29" spans="2:6" ht="63">
       <c r="B29" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C29" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="D29" s="4" t="s">
         <v>71</v>
       </c>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+    </row>
+    <row r="30" spans="2:6" ht="47.25">
+      <c r="B30" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+    </row>
+    <row r="31" spans="2:6" ht="47.25">
+      <c r="B31" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E31" s="9"/>
+      <c r="F31" s="7"/>
+    </row>
+    <row r="32" spans="2:6" ht="63">
+      <c r="B32" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E32" s="9"/>
+      <c r="F32" s="7"/>
+    </row>
+    <row r="33" spans="2:6" ht="47.25">
+      <c r="B33" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E33" s="9"/>
+      <c r="F33" s="7"/>
+    </row>
+    <row r="34" spans="2:6">
+      <c r="B34" s="5"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>